<commit_message>
feat: complete section 3 - render pdf report & refactor code
</commit_message>
<xml_diff>
--- a/reports/excel_reports/analysis_results.xlsx
+++ b/reports/excel_reports/analysis_results.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,21 +448,41 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-01</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-02</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,41 +519,51 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>/checkout</t>
+          <t>/about</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>/about</t>
+          <t>/product</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>/product</t>
+          <t>/checkout</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
+          <t>/contact</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
           <t>/home</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>2</v>
+      <c r="B6" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,19 +586,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Average Session Duration (s)</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Average Session Duration (s)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>[np.float64(11208.0)]</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              duration
+session_id            
+5001        281.142857
+5002        319.000000
+5003        307.681818
+5004        286.952381
+5005        366.368421</t>
         </is>
       </c>
     </row>

</xml_diff>